<commit_message>
Correct Persian Data Format
The persian date in Format year.month is will be used from this point.
e.g. 1369.02
for quarterly data use the last moth of season : 69.03 69.06 69.09 69.12
</commit_message>
<xml_diff>
--- a/Matlab/ForeCasteToolbox/Input/Data.xlsx
+++ b/Matlab/ForeCasteToolbox/Input/Data.xlsx
@@ -2321,7 +2321,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2418,7 +2418,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="7">
-        <v>1369.1</v>
+        <v>1369.03</v>
       </c>
       <c r="B3" s="10">
         <v>2.3666666666666698</v>
@@ -2459,7 +2459,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="7">
-        <v>1369.2</v>
+        <v>1369.06</v>
       </c>
       <c r="B4" s="10">
         <v>2.43333333333333</v>
@@ -2500,7 +2500,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="7">
-        <v>1369.3</v>
+        <v>1369.09</v>
       </c>
       <c r="B5" s="10">
         <v>2.56666666666667</v>
@@ -2541,7 +2541,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="7">
-        <v>1369.4</v>
+        <v>1369.12</v>
       </c>
       <c r="B6" s="10">
         <v>2.7</v>
@@ -2582,8 +2582,8 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1">
-        <f t="shared" ref="A7:A70" si="0">IF(A6-ROUND(A6,0)&gt;0.31,A3+1,A6+0.1)</f>
-        <v>1370.1</v>
+        <f>IF(A6-ROUND(A6,0)&gt;0.1,A3+1,A6+0.03)</f>
+        <v>1370.03</v>
       </c>
       <c r="B7" s="10">
         <v>2.8666666666666698</v>
@@ -2624,8 +2624,8 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="1">
-        <f t="shared" si="0"/>
-        <v>1370.1999999999998</v>
+        <f t="shared" ref="A8:A71" si="0">IF(A7-ROUND(A7,0)&gt;0.1,A4+1,A7+0.03)</f>
+        <v>1370.06</v>
       </c>
       <c r="B8" s="10">
         <v>3</v>
@@ -2667,7 +2667,7 @@
     <row r="9" spans="1:13">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
-        <v>1370.2999999999997</v>
+        <v>1370.09</v>
       </c>
       <c r="B9" s="10">
         <v>3.2333333333333298</v>
@@ -2709,7 +2709,7 @@
     <row r="10" spans="1:13">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
-        <v>1370.3999999999996</v>
+        <v>1370.12</v>
       </c>
       <c r="B10" s="10">
         <v>3.5</v>
@@ -2751,7 +2751,7 @@
     <row r="11" spans="1:13">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
-        <v>1371.1</v>
+        <v>1371.03</v>
       </c>
       <c r="B11" s="10">
         <v>3.56666666666667</v>
@@ -2793,7 +2793,7 @@
     <row r="12" spans="1:13">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
-        <v>1371.1999999999998</v>
+        <v>1371.06</v>
       </c>
       <c r="B12" s="10">
         <v>3.6333333333333302</v>
@@ -2835,7 +2835,7 @@
     <row r="13" spans="1:13">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
-        <v>1371.2999999999997</v>
+        <v>1371.09</v>
       </c>
       <c r="B13" s="10">
         <v>3.9</v>
@@ -2877,7 +2877,7 @@
     <row r="14" spans="1:13">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
-        <v>1371.3999999999996</v>
+        <v>1371.12</v>
       </c>
       <c r="B14" s="10">
         <v>4.1333333333333302</v>
@@ -2919,7 +2919,7 @@
     <row r="15" spans="1:13">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
-        <v>1372.1</v>
+        <v>1372.03</v>
       </c>
       <c r="B15" s="10">
         <v>4.3</v>
@@ -2961,7 +2961,7 @@
     <row r="16" spans="1:13">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
-        <v>1372.1999999999998</v>
+        <v>1372.06</v>
       </c>
       <c r="B16" s="10">
         <v>4.56666666666667</v>
@@ -3003,7 +3003,7 @@
     <row r="17" spans="1:13">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
-        <v>1372.2999999999997</v>
+        <v>1372.09</v>
       </c>
       <c r="B17" s="10">
         <v>4.9666666666666703</v>
@@ -3045,7 +3045,7 @@
     <row r="18" spans="1:13">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
-        <v>1372.3999999999996</v>
+        <v>1372.12</v>
       </c>
       <c r="B18" s="10">
         <v>5.4</v>
@@ -3087,7 +3087,7 @@
     <row r="19" spans="1:13">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
-        <v>1373.1</v>
+        <v>1373.03</v>
       </c>
       <c r="B19" s="10">
         <v>5.7333333333333298</v>
@@ -3129,7 +3129,7 @@
     <row r="20" spans="1:13">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
-        <v>1373.1999999999998</v>
+        <v>1373.06</v>
       </c>
       <c r="B20" s="10">
         <v>6.2333333333333298</v>
@@ -3171,7 +3171,7 @@
     <row r="21" spans="1:13">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
-        <v>1373.2999999999997</v>
+        <v>1373.09</v>
       </c>
       <c r="B21" s="10">
         <v>7</v>
@@ -3213,7 +3213,7 @@
     <row r="22" spans="1:13">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
-        <v>1373.3999999999996</v>
+        <v>1373.12</v>
       </c>
       <c r="B22" s="10">
         <v>8.4</v>
@@ -3255,7 +3255,7 @@
     <row r="23" spans="1:13">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
-        <v>1374.1</v>
+        <v>1374.03</v>
       </c>
       <c r="B23" s="10">
         <v>8.6666666666666696</v>
@@ -3297,7 +3297,7 @@
     <row r="24" spans="1:13">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
-        <v>1374.1999999999998</v>
+        <v>1374.06</v>
       </c>
       <c r="B24" s="10">
         <v>9.2333333333333307</v>
@@ -3339,7 +3339,7 @@
     <row r="25" spans="1:13">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
-        <v>1374.2999999999997</v>
+        <v>1374.09</v>
       </c>
       <c r="B25" s="10">
         <v>10</v>
@@ -3381,7 +3381,7 @@
     <row r="26" spans="1:13">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
-        <v>1374.3999999999996</v>
+        <v>1374.12</v>
       </c>
       <c r="B26" s="10">
         <v>10.8</v>
@@ -3423,7 +3423,7 @@
     <row r="27" spans="1:13">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
-        <v>1375.1</v>
+        <v>1375.03</v>
       </c>
       <c r="B27" s="10">
         <v>10.866666666666699</v>
@@ -3465,7 +3465,7 @@
     <row r="28" spans="1:13">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
-        <v>1375.1999999999998</v>
+        <v>1375.06</v>
       </c>
       <c r="B28" s="10">
         <v>11.3</v>
@@ -3507,7 +3507,7 @@
     <row r="29" spans="1:13">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
-        <v>1375.2999999999997</v>
+        <v>1375.09</v>
       </c>
       <c r="B29" s="10">
         <v>11.8333333333333</v>
@@ -3549,7 +3549,7 @@
     <row r="30" spans="1:13">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
-        <v>1375.3999999999996</v>
+        <v>1375.12</v>
       </c>
       <c r="B30" s="10">
         <v>12.6</v>
@@ -3591,7 +3591,7 @@
     <row r="31" spans="1:13">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
-        <v>1376.1</v>
+        <v>1376.03</v>
       </c>
       <c r="B31" s="10">
         <v>12.866666666666699</v>
@@ -3633,7 +3633,7 @@
     <row r="32" spans="1:13">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
-        <v>1376.1999999999998</v>
+        <v>1376.06</v>
       </c>
       <c r="B32" s="10">
         <v>13.133333333333301</v>
@@ -3675,7 +3675,7 @@
     <row r="33" spans="1:13">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
-        <v>1376.2999999999997</v>
+        <v>1376.09</v>
       </c>
       <c r="B33" s="10">
         <v>13.9333333333333</v>
@@ -3717,7 +3717,7 @@
     <row r="34" spans="1:13">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
-        <v>1376.3999999999996</v>
+        <v>1376.12</v>
       </c>
       <c r="B34" s="10">
         <v>14.8</v>
@@ -3759,7 +3759,7 @@
     <row r="35" spans="1:13">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
-        <v>1377.1</v>
+        <v>1377.03</v>
       </c>
       <c r="B35" s="10">
         <v>15.0666666666667</v>
@@ -3801,7 +3801,7 @@
     <row r="36" spans="1:13">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
-        <v>1377.1999999999998</v>
+        <v>1377.06</v>
       </c>
       <c r="B36" s="10">
         <v>15.6666666666667</v>
@@ -3843,7 +3843,7 @@
     <row r="37" spans="1:13">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
-        <v>1377.2999999999997</v>
+        <v>1377.09</v>
       </c>
       <c r="B37" s="10">
         <v>16.533333333333299</v>
@@ -3885,7 +3885,7 @@
     <row r="38" spans="1:13">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
-        <v>1377.3999999999996</v>
+        <v>1377.12</v>
       </c>
       <c r="B38" s="10">
         <v>18</v>
@@ -3927,7 +3927,7 @@
     <row r="39" spans="1:13">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
-        <v>1378.1</v>
+        <v>1378.03</v>
       </c>
       <c r="B39" s="10">
         <v>18.133333333333301</v>
@@ -3969,7 +3969,7 @@
     <row r="40" spans="1:13">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
-        <v>1378.1999999999998</v>
+        <v>1378.06</v>
       </c>
       <c r="B40" s="10">
         <v>18.733333333333299</v>
@@ -4011,7 +4011,7 @@
     <row r="41" spans="1:13">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
-        <v>1378.2999999999997</v>
+        <v>1378.09</v>
       </c>
       <c r="B41" s="10">
         <v>19.7</v>
@@ -4053,7 +4053,7 @@
     <row r="42" spans="1:13">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
-        <v>1378.3999999999996</v>
+        <v>1378.12</v>
       </c>
       <c r="B42" s="10">
         <v>20.3</v>
@@ -4095,7 +4095,7 @@
     <row r="43" spans="1:13">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
-        <v>1379.1</v>
+        <v>1379.03</v>
       </c>
       <c r="B43" s="10">
         <v>20.533333333333299</v>
@@ -4137,7 +4137,7 @@
     <row r="44" spans="1:13">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
-        <v>1379.1999999999998</v>
+        <v>1379.06</v>
       </c>
       <c r="B44" s="10">
         <v>21.1666666666667</v>
@@ -4179,7 +4179,7 @@
     <row r="45" spans="1:13">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
-        <v>1379.2999999999997</v>
+        <v>1379.09</v>
       </c>
       <c r="B45" s="10">
         <v>21.866666666666699</v>
@@ -4221,7 +4221,7 @@
     <row r="46" spans="1:13">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
-        <v>1379.3999999999996</v>
+        <v>1379.12</v>
       </c>
       <c r="B46" s="10">
         <v>22.633333333333301</v>
@@ -4263,7 +4263,7 @@
     <row r="47" spans="1:13">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
-        <v>1380.1</v>
+        <v>1380.03</v>
       </c>
       <c r="B47" s="10">
         <v>22.966666666666701</v>
@@ -4305,7 +4305,7 @@
     <row r="48" spans="1:13">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
-        <v>1380.1999999999998</v>
+        <v>1380.06</v>
       </c>
       <c r="B48" s="10">
         <v>23.433333333333302</v>
@@ -4347,7 +4347,7 @@
     <row r="49" spans="1:13">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
-        <v>1380.2999999999997</v>
+        <v>1380.09</v>
       </c>
       <c r="B49" s="10">
         <v>24.433333333333302</v>
@@ -4389,7 +4389,7 @@
     <row r="50" spans="1:13">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
-        <v>1380.3999999999996</v>
+        <v>1380.12</v>
       </c>
       <c r="B50" s="10">
         <v>25.8333333333333</v>
@@ -4431,7 +4431,7 @@
     <row r="51" spans="1:13">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
-        <v>1381.1</v>
+        <v>1381.03</v>
       </c>
       <c r="B51" s="10">
         <v>26.5</v>
@@ -4473,7 +4473,7 @@
     <row r="52" spans="1:13">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
-        <v>1381.1999999999998</v>
+        <v>1381.06</v>
       </c>
       <c r="B52" s="10">
         <v>27.233333333333299</v>
@@ -4515,7 +4515,7 @@
     <row r="53" spans="1:13">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
-        <v>1381.2999999999997</v>
+        <v>1381.09</v>
       </c>
       <c r="B53" s="10">
         <v>28.766666666666701</v>
@@ -4557,7 +4557,7 @@
     <row r="54" spans="1:13">
       <c r="A54" s="1">
         <f t="shared" si="0"/>
-        <v>1381.3999999999996</v>
+        <v>1381.12</v>
       </c>
       <c r="B54" s="10">
         <v>30.133333333333301</v>
@@ -4599,7 +4599,7 @@
     <row r="55" spans="1:13">
       <c r="A55" s="1">
         <f t="shared" si="0"/>
-        <v>1382.1</v>
+        <v>1382.03</v>
       </c>
       <c r="B55" s="10">
         <v>30.766666666666701</v>
@@ -4641,7 +4641,7 @@
     <row r="56" spans="1:13">
       <c r="A56" s="1">
         <f t="shared" si="0"/>
-        <v>1382.1999999999998</v>
+        <v>1382.06</v>
       </c>
       <c r="B56" s="10">
         <v>31.5</v>
@@ -4683,7 +4683,7 @@
     <row r="57" spans="1:13">
       <c r="A57" s="1">
         <f t="shared" si="0"/>
-        <v>1382.2999999999997</v>
+        <v>1382.09</v>
       </c>
       <c r="B57" s="10">
         <v>32.799999999999997</v>
@@ -4725,7 +4725,7 @@
     <row r="58" spans="1:13">
       <c r="A58" s="1">
         <f t="shared" si="0"/>
-        <v>1382.3999999999996</v>
+        <v>1382.12</v>
       </c>
       <c r="B58" s="10">
         <v>34.533333333333303</v>
@@ -4767,7 +4767,7 @@
     <row r="59" spans="1:13">
       <c r="A59" s="1">
         <f t="shared" si="0"/>
-        <v>1383.1</v>
+        <v>1383.03</v>
       </c>
       <c r="B59" s="10">
         <v>35.566666666666698</v>
@@ -4809,7 +4809,7 @@
     <row r="60" spans="1:13">
       <c r="A60" s="1">
         <f t="shared" si="0"/>
-        <v>1383.1999999999998</v>
+        <v>1383.06</v>
       </c>
       <c r="B60" s="10">
         <v>36.433333333333302</v>
@@ -4851,7 +4851,7 @@
     <row r="61" spans="1:13">
       <c r="A61" s="1">
         <f t="shared" si="0"/>
-        <v>1383.2999999999997</v>
+        <v>1383.09</v>
       </c>
       <c r="B61" s="10">
         <v>37.799999999999997</v>
@@ -4893,7 +4893,7 @@
     <row r="62" spans="1:13">
       <c r="A62" s="1">
         <f t="shared" si="0"/>
-        <v>1383.3999999999996</v>
+        <v>1383.12</v>
       </c>
       <c r="B62" s="10">
         <v>39.466666666666697</v>
@@ -4935,7 +4935,7 @@
     <row r="63" spans="1:13">
       <c r="A63" s="1">
         <f t="shared" si="0"/>
-        <v>1384.1</v>
+        <v>1384.03</v>
       </c>
       <c r="B63" s="10">
         <v>39.033333333333303</v>
@@ -4977,7 +4977,7 @@
     <row r="64" spans="1:13">
       <c r="A64" s="1">
         <f t="shared" si="0"/>
-        <v>1384.1999999999998</v>
+        <v>1384.06</v>
       </c>
       <c r="B64" s="10">
         <v>39.799999999999997</v>
@@ -5019,7 +5019,7 @@
     <row r="65" spans="1:13">
       <c r="A65" s="1">
         <f t="shared" si="0"/>
-        <v>1384.2999999999997</v>
+        <v>1384.09</v>
       </c>
       <c r="B65" s="10">
         <v>40.966666666666697</v>
@@ -5061,7 +5061,7 @@
     <row r="66" spans="1:13">
       <c r="A66" s="1">
         <f t="shared" si="0"/>
-        <v>1384.3999999999996</v>
+        <v>1384.12</v>
       </c>
       <c r="B66" s="10">
         <v>42.3</v>
@@ -5103,7 +5103,7 @@
     <row r="67" spans="1:13">
       <c r="A67" s="1">
         <f t="shared" si="0"/>
-        <v>1385.1</v>
+        <v>1385.03</v>
       </c>
       <c r="B67" s="10">
         <v>43.3</v>
@@ -5145,7 +5145,7 @@
     <row r="68" spans="1:13">
       <c r="A68" s="1">
         <f t="shared" si="0"/>
-        <v>1385.1999999999998</v>
+        <v>1385.06</v>
       </c>
       <c r="B68" s="10">
         <v>45.133333333333297</v>
@@ -5187,7 +5187,7 @@
     <row r="69" spans="1:13">
       <c r="A69" s="1">
         <f t="shared" si="0"/>
-        <v>1385.2999999999997</v>
+        <v>1385.09</v>
       </c>
       <c r="B69" s="10">
         <v>47.466666666666697</v>
@@ -5229,7 +5229,7 @@
     <row r="70" spans="1:13">
       <c r="A70" s="1">
         <f t="shared" si="0"/>
-        <v>1385.3999999999996</v>
+        <v>1385.12</v>
       </c>
       <c r="B70" s="10">
         <v>49.266666666666701</v>
@@ -5270,8 +5270,8 @@
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="1">
-        <f t="shared" ref="A71:A124" si="1">IF(A70-ROUND(A70,0)&gt;0.31,A67+1,A70+0.1)</f>
-        <v>1386.1</v>
+        <f t="shared" si="0"/>
+        <v>1386.03</v>
       </c>
       <c r="B71" s="10">
         <v>50.8333333333333</v>
@@ -5312,8 +5312,8 @@
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="1">
-        <f t="shared" si="1"/>
-        <v>1386.1999999999998</v>
+        <f t="shared" ref="A72:A124" si="1">IF(A71-ROUND(A71,0)&gt;0.1,A68+1,A71+0.03)</f>
+        <v>1386.06</v>
       </c>
       <c r="B72" s="10">
         <v>53.7</v>
@@ -5355,7 +5355,7 @@
     <row r="73" spans="1:13">
       <c r="A73" s="1">
         <f t="shared" si="1"/>
-        <v>1386.2999999999997</v>
+        <v>1386.09</v>
       </c>
       <c r="B73" s="10">
         <v>57.266666666666701</v>
@@ -5397,7 +5397,7 @@
     <row r="74" spans="1:13">
       <c r="A74" s="1">
         <f t="shared" si="1"/>
-        <v>1386.3999999999996</v>
+        <v>1386.12</v>
       </c>
       <c r="B74" s="10">
         <v>61.733333333333299</v>
@@ -5439,7 +5439,7 @@
     <row r="75" spans="1:13">
       <c r="A75" s="1">
         <f t="shared" si="1"/>
-        <v>1387.1</v>
+        <v>1387.03</v>
       </c>
       <c r="B75" s="10">
         <v>64.933333333333294</v>
@@ -5481,7 +5481,7 @@
     <row r="76" spans="1:13">
       <c r="A76" s="1">
         <f t="shared" si="1"/>
-        <v>1387.1999999999998</v>
+        <v>1387.06</v>
       </c>
       <c r="B76" s="10">
         <v>68.733333333333306</v>
@@ -5523,7 +5523,7 @@
     <row r="77" spans="1:13">
       <c r="A77" s="1">
         <f t="shared" si="1"/>
-        <v>1387.2999999999997</v>
+        <v>1387.09</v>
       </c>
       <c r="B77" s="10">
         <v>69.099999999999994</v>
@@ -5565,7 +5565,7 @@
     <row r="78" spans="1:13">
       <c r="A78" s="1">
         <f t="shared" si="1"/>
-        <v>1387.3999999999996</v>
+        <v>1387.12</v>
       </c>
       <c r="B78" s="10">
         <v>71</v>
@@ -5607,7 +5607,7 @@
     <row r="79" spans="1:13">
       <c r="A79" s="1">
         <f t="shared" si="1"/>
-        <v>1388.1</v>
+        <v>1388.03</v>
       </c>
       <c r="B79" s="10">
         <v>72.766666666666694</v>
@@ -5649,7 +5649,7 @@
     <row r="80" spans="1:13">
       <c r="A80" s="1">
         <f t="shared" si="1"/>
-        <v>1388.1999999999998</v>
+        <v>1388.06</v>
       </c>
       <c r="B80" s="10">
         <v>73.866666666666703</v>
@@ -5691,7 +5691,7 @@
     <row r="81" spans="1:13">
       <c r="A81" s="1">
         <f t="shared" si="1"/>
-        <v>1388.2999999999997</v>
+        <v>1388.09</v>
       </c>
       <c r="B81" s="10">
         <v>75.400000000000006</v>
@@ -5733,7 +5733,7 @@
     <row r="82" spans="1:13" s="9" customFormat="1">
       <c r="A82" s="1">
         <f t="shared" si="1"/>
-        <v>1388.3999999999996</v>
+        <v>1388.12</v>
       </c>
       <c r="B82" s="10">
         <v>77.599999999999994</v>
@@ -5775,7 +5775,7 @@
     <row r="83" spans="1:13">
       <c r="A83" s="1">
         <f t="shared" si="1"/>
-        <v>1389.1</v>
+        <v>1389.03</v>
       </c>
       <c r="B83" s="10">
         <v>79.766666666666694</v>
@@ -5817,7 +5817,7 @@
     <row r="84" spans="1:13">
       <c r="A84" s="1">
         <f t="shared" si="1"/>
-        <v>1389.1999999999998</v>
+        <v>1389.06</v>
       </c>
       <c r="B84" s="10">
         <v>83.033333333333402</v>
@@ -5859,7 +5859,7 @@
     <row r="85" spans="1:13">
       <c r="A85" s="1">
         <f t="shared" si="1"/>
-        <v>1389.2999999999997</v>
+        <v>1389.09</v>
       </c>
       <c r="B85" s="10">
         <v>88.866666666666703</v>
@@ -5901,7 +5901,7 @@
     <row r="86" spans="1:13" s="9" customFormat="1">
       <c r="A86" s="1">
         <f t="shared" si="1"/>
-        <v>1389.3999999999996</v>
+        <v>1389.12</v>
       </c>
       <c r="B86" s="10">
         <v>94.433333333333294</v>
@@ -5943,7 +5943,7 @@
     <row r="87" spans="1:13">
       <c r="A87" s="1">
         <f t="shared" si="1"/>
-        <v>1390.1</v>
+        <v>1390.03</v>
       </c>
       <c r="B87" s="10">
         <v>97.1666666666667</v>
@@ -5985,7 +5985,7 @@
     <row r="88" spans="1:13">
       <c r="A88" s="1">
         <f t="shared" si="1"/>
-        <v>1390.1999999999998</v>
+        <v>1390.06</v>
       </c>
       <c r="B88" s="10">
         <v>101.3</v>
@@ -6027,7 +6027,7 @@
     <row r="89" spans="1:13">
       <c r="A89" s="1">
         <f t="shared" si="1"/>
-        <v>1390.2999999999997</v>
+        <v>1390.09</v>
       </c>
       <c r="B89" s="10">
         <v>107.133333333333</v>
@@ -6069,7 +6069,7 @@
     <row r="90" spans="1:13">
       <c r="A90" s="1">
         <f t="shared" si="1"/>
-        <v>1390.3999999999996</v>
+        <v>1390.12</v>
       </c>
       <c r="B90" s="10">
         <v>115.033333333333</v>
@@ -6111,7 +6111,7 @@
     <row r="91" spans="1:13">
       <c r="A91" s="1">
         <f t="shared" si="1"/>
-        <v>1391.1</v>
+        <v>1391.03</v>
       </c>
       <c r="B91" s="10">
         <v>121.76666666666701</v>
@@ -6153,7 +6153,7 @@
     <row r="92" spans="1:13">
       <c r="A92" s="1">
         <f t="shared" si="1"/>
-        <v>1391.1999999999998</v>
+        <v>1391.06</v>
       </c>
       <c r="B92" s="10">
         <v>135.86666666666699</v>
@@ -6195,7 +6195,7 @@
     <row r="93" spans="1:13">
       <c r="A93" s="1">
         <f t="shared" si="1"/>
-        <v>1391.2999999999997</v>
+        <v>1391.09</v>
       </c>
       <c r="B93" s="10">
         <v>149.5</v>
@@ -6237,7 +6237,7 @@
     <row r="94" spans="1:13">
       <c r="A94" s="1">
         <f t="shared" si="1"/>
-        <v>1391.3999999999996</v>
+        <v>1391.12</v>
       </c>
       <c r="B94" s="10">
         <v>164.5</v>
@@ -6279,7 +6279,7 @@
     <row r="95" spans="1:13">
       <c r="A95" s="1">
         <f t="shared" si="1"/>
-        <v>1392.1</v>
+        <v>1392.03</v>
       </c>
       <c r="B95" s="10">
         <v>174</v>
@@ -6321,7 +6321,7 @@
     <row r="96" spans="1:13">
       <c r="A96" s="1">
         <f t="shared" si="1"/>
-        <v>1392.1999999999998</v>
+        <v>1392.06</v>
       </c>
       <c r="B96" s="10">
         <v>180.2</v>
@@ -6363,7 +6363,7 @@
     <row r="97" spans="1:13" s="9" customFormat="1">
       <c r="A97" s="1">
         <f t="shared" si="1"/>
-        <v>1392.2999999999997</v>
+        <v>1392.09</v>
       </c>
       <c r="B97" s="10">
         <v>184.8</v>
@@ -6405,7 +6405,7 @@
     <row r="98" spans="1:13">
       <c r="A98" s="1">
         <f t="shared" si="1"/>
-        <v>1392.3999999999996</v>
+        <v>1392.12</v>
       </c>
       <c r="B98" s="10">
         <v>191.1</v>
@@ -6447,7 +6447,7 @@
     <row r="99" spans="1:13">
       <c r="A99" s="1">
         <f t="shared" si="1"/>
-        <v>1393.1</v>
+        <v>1393.03</v>
       </c>
       <c r="B99" s="10">
         <v>199.4</v>
@@ -6489,7 +6489,7 @@
     <row r="100" spans="1:13">
       <c r="A100" s="1">
         <f t="shared" si="1"/>
-        <v>1393.1999999999998</v>
+        <v>1393.06</v>
       </c>
       <c r="B100" s="10">
         <v>208.1</v>
@@ -6531,7 +6531,7 @@
     <row r="101" spans="1:13">
       <c r="A101" s="1">
         <f t="shared" si="1"/>
-        <v>1393.2999999999997</v>
+        <v>1393.09</v>
       </c>
       <c r="B101" s="14">
         <v>214.4</v>
@@ -6573,7 +6573,7 @@
     <row r="102" spans="1:13">
       <c r="A102" s="1">
         <f t="shared" si="1"/>
-        <v>1393.3999999999996</v>
+        <v>1393.12</v>
       </c>
       <c r="B102" s="10">
         <v>222.5</v>
@@ -6615,7 +6615,7 @@
     <row r="103" spans="1:13">
       <c r="A103" s="1">
         <f t="shared" si="1"/>
-        <v>1394.1</v>
+        <v>1394.03</v>
       </c>
       <c r="B103" s="10">
         <v>225.7</v>
@@ -6657,7 +6657,7 @@
     <row r="104" spans="1:13">
       <c r="A104" s="1">
         <f t="shared" si="1"/>
-        <v>1394.1999999999998</v>
+        <v>1394.06</v>
       </c>
       <c r="B104" s="10">
         <v>231.6</v>
@@ -6699,7 +6699,7 @@
     <row r="105" spans="1:13">
       <c r="A105" s="1">
         <f t="shared" si="1"/>
-        <v>1394.2999999999997</v>
+        <v>1394.09</v>
       </c>
       <c r="B105" s="10">
         <v>234.8</v>
@@ -6741,7 +6741,7 @@
     <row r="106" spans="1:13">
       <c r="A106" s="1">
         <f t="shared" si="1"/>
-        <v>1394.3999999999996</v>
+        <v>1394.12</v>
       </c>
       <c r="B106" s="10">
         <v>240.9</v>
@@ -6783,7 +6783,7 @@
     <row r="107" spans="1:13">
       <c r="A107" s="1">
         <f t="shared" si="1"/>
-        <v>1395.1</v>
+        <v>1395.03</v>
       </c>
       <c r="B107" s="10">
         <v>247.1</v>
@@ -6825,7 +6825,7 @@
     <row r="108" spans="1:13">
       <c r="A108" s="1">
         <f t="shared" si="1"/>
-        <v>1395.1999999999998</v>
+        <v>1395.06</v>
       </c>
       <c r="L108" s="10">
         <v>1</v>
@@ -6837,7 +6837,7 @@
     <row r="109" spans="1:13">
       <c r="A109" s="1">
         <f t="shared" si="1"/>
-        <v>1395.2999999999997</v>
+        <v>1395.09</v>
       </c>
       <c r="L109" s="10">
         <v>1</v>
@@ -6849,7 +6849,7 @@
     <row r="110" spans="1:13">
       <c r="A110" s="1">
         <f t="shared" si="1"/>
-        <v>1395.3999999999996</v>
+        <v>1395.12</v>
       </c>
       <c r="L110" s="10">
         <v>1</v>
@@ -6861,7 +6861,7 @@
     <row r="111" spans="1:13">
       <c r="A111" s="1">
         <f t="shared" si="1"/>
-        <v>1396.1</v>
+        <v>1396.03</v>
       </c>
       <c r="L111" s="10">
         <v>1</v>
@@ -6873,7 +6873,7 @@
     <row r="112" spans="1:13">
       <c r="A112" s="1">
         <f t="shared" si="1"/>
-        <v>1396.1999999999998</v>
+        <v>1396.06</v>
       </c>
       <c r="L112" s="10">
         <v>1</v>
@@ -6885,7 +6885,7 @@
     <row r="113" spans="1:13">
       <c r="A113" s="1">
         <f t="shared" si="1"/>
-        <v>1396.2999999999997</v>
+        <v>1396.09</v>
       </c>
       <c r="L113" s="10">
         <v>1</v>
@@ -6897,7 +6897,7 @@
     <row r="114" spans="1:13">
       <c r="A114" s="1">
         <f t="shared" si="1"/>
-        <v>1396.3999999999996</v>
+        <v>1396.12</v>
       </c>
       <c r="L114" s="10">
         <v>1</v>
@@ -6909,7 +6909,7 @@
     <row r="115" spans="1:13">
       <c r="A115" s="1">
         <f t="shared" si="1"/>
-        <v>1397.1</v>
+        <v>1397.03</v>
       </c>
       <c r="L115" s="10">
         <v>1</v>
@@ -6921,7 +6921,7 @@
     <row r="116" spans="1:13">
       <c r="A116" s="1">
         <f t="shared" si="1"/>
-        <v>1397.1999999999998</v>
+        <v>1397.06</v>
       </c>
       <c r="L116" s="10">
         <v>1</v>
@@ -6933,7 +6933,7 @@
     <row r="117" spans="1:13">
       <c r="A117" s="1">
         <f t="shared" si="1"/>
-        <v>1397.2999999999997</v>
+        <v>1397.09</v>
       </c>
       <c r="L117" s="10">
         <v>1</v>
@@ -6945,7 +6945,7 @@
     <row r="118" spans="1:13">
       <c r="A118" s="1">
         <f t="shared" si="1"/>
-        <v>1397.3999999999996</v>
+        <v>1397.12</v>
       </c>
       <c r="L118" s="10">
         <v>1</v>
@@ -6957,7 +6957,7 @@
     <row r="119" spans="1:13">
       <c r="A119" s="1">
         <f t="shared" si="1"/>
-        <v>1398.1</v>
+        <v>1398.03</v>
       </c>
       <c r="L119" s="10">
         <v>1</v>
@@ -6969,7 +6969,7 @@
     <row r="120" spans="1:13">
       <c r="A120" s="1">
         <f t="shared" si="1"/>
-        <v>1398.1999999999998</v>
+        <v>1398.06</v>
       </c>
       <c r="L120" s="10">
         <v>1</v>
@@ -6981,7 +6981,7 @@
     <row r="121" spans="1:13">
       <c r="A121" s="1">
         <f t="shared" si="1"/>
-        <v>1398.2999999999997</v>
+        <v>1398.09</v>
       </c>
       <c r="L121" s="10">
         <v>1</v>
@@ -6993,7 +6993,7 @@
     <row r="122" spans="1:13">
       <c r="A122" s="1">
         <f t="shared" si="1"/>
-        <v>1398.3999999999996</v>
+        <v>1398.12</v>
       </c>
       <c r="L122" s="10">
         <v>1</v>
@@ -7005,7 +7005,7 @@
     <row r="123" spans="1:13">
       <c r="A123" s="1">
         <f t="shared" si="1"/>
-        <v>1399.1</v>
+        <v>1399.03</v>
       </c>
       <c r="L123" s="10">
         <v>1</v>
@@ -7017,7 +7017,7 @@
     <row r="124" spans="1:13">
       <c r="A124" s="1">
         <f t="shared" si="1"/>
-        <v>1399.1999999999998</v>
+        <v>1399.06</v>
       </c>
     </row>
   </sheetData>
@@ -58922,7 +58922,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>